<commit_message>
[api]  more detailed errors when importing meter readings
</commit_message>
<xml_diff>
--- a/web/elec/fixtures/points-de-recharge-errors.xlsx
+++ b/web/elec/fixtures/points-de-recharge-errors.xlsx
@@ -140,16 +140,16 @@
     <t>NOT A NUMBER</t>
   </si>
   <si>
-    <t>FRELCEJ37W</t>
+    <t>ABCDE</t>
   </si>
   <si>
-    <t>FRELCET4BC</t>
+    <t>FGHIJ</t>
   </si>
   <si>
-    <t>FRELCEGK4C</t>
+    <t>KLMNO</t>
   </si>
   <si>
-    <t>FRELCETTJ5</t>
+    <t>PQRST</t>
   </si>
 </sst>
 </file>

</xml_diff>